<commit_message>
Changes analysis, tables and graphs
</commit_message>
<xml_diff>
--- a/output/ajuste2016.xlsx
+++ b/output/ajuste2016.xlsx
@@ -434,22 +434,22 @@
         </is>
       </c>
       <c r="B3">
-        <v>-2328.346493560737</v>
+        <v>-2328.346493560788</v>
       </c>
       <c r="C3">
-        <v>4024.079716035722</v>
+        <v>4024.079716055674</v>
       </c>
       <c r="D3">
-        <v>480.3115075978617</v>
+        <v>480.3115075978895</v>
       </c>
       <c r="E3">
         <v>31</v>
       </c>
       <c r="F3">
-        <v>4718.692987121473</v>
+        <v>4718.692987121575</v>
       </c>
       <c r="G3">
-        <v>4846.962525798147</v>
+        <v>4846.962525798249</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -462,22 +462,22 @@
         </is>
       </c>
       <c r="B4">
-        <v>-2227.756688798213</v>
+        <v>-2209.92758755932</v>
       </c>
       <c r="C4">
-        <v>3162.806364920602</v>
+        <v>3199.50935591981</v>
       </c>
       <c r="D4">
-        <v>415.1135649546665</v>
+        <v>408.7700485178675</v>
       </c>
       <c r="E4">
         <v>47</v>
       </c>
       <c r="F4">
-        <v>4549.513377596425</v>
+        <v>4513.855175118641</v>
       </c>
       <c r="G4">
-        <v>4743.986549138478</v>
+        <v>4708.328346660694</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -490,22 +490,22 @@
         </is>
       </c>
       <c r="B5">
-        <v>-2187.061846107358</v>
+        <v>-2198.768944509708</v>
       </c>
       <c r="C5">
-        <v>936.9469705879393</v>
+        <v>1310.539557061597</v>
       </c>
       <c r="D5">
-        <v>384.0042094792408</v>
+        <v>423.0238552106839</v>
       </c>
       <c r="E5">
         <v>63</v>
       </c>
       <c r="F5">
-        <v>4500.123692214715</v>
+        <v>4523.537889019416</v>
       </c>
       <c r="G5">
-        <v>4760.800496622148</v>
+        <v>4784.214693426849</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -518,22 +518,22 @@
         </is>
       </c>
       <c r="B6">
-        <v>-2079.942253226425</v>
+        <v>-2102.035380288189</v>
       </c>
       <c r="C6">
-        <v>818.1650730581771</v>
+        <v>1968.34373054423</v>
       </c>
       <c r="D6">
-        <v>323.4159110210288</v>
+        <v>336.241794453155</v>
       </c>
       <c r="E6">
         <v>79</v>
       </c>
       <c r="F6">
-        <v>4317.884506452851</v>
+        <v>4362.070760576378</v>
       </c>
       <c r="G6">
-        <v>4644.764943725663</v>
+        <v>4688.951197849191</v>
       </c>
       <c r="H6">
         <v>0</v>

</xml_diff>